<commit_message>
Add email address to voter record.
</commit_message>
<xml_diff>
--- a/elections/exports/event_data_template.xlsx
+++ b/elections/exports/event_data_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t xml:space="preserve">property</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">writein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
   </si>
   <si>
     <t xml:space="preserve">voteid</t>
@@ -224,11 +227,11 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
@@ -295,10 +298,10 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="211"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10"/>
   </cols>
@@ -355,16 +358,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
   </cols>
@@ -413,21 +416,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -443,9 +447,10 @@
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -462,13 +467,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="10"/>
   </cols>
@@ -478,13 +483,13 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -607,14 +612,14 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>